<commit_message>
Start of Unit Value Factor
</commit_message>
<xml_diff>
--- a/GD-Docs/CodeCamelUnitProto.xlsx
+++ b/GD-Docs/CodeCamelUnitProto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phile\Documents\GitKraken\CodeCamelV2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phile\Documents\GitKraken\CodeCamelV2\GD-Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53630311-947C-4573-99BC-33FC60F7DA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE902553-4E9F-45BF-8C8B-00334AC26186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B6672DD-3FD7-46DC-9F9A-0AB6F6387CA9}"/>
+    <workbookView xWindow="11988" yWindow="1728" windowWidth="11268" windowHeight="8964" xr2:uid="{6B6672DD-3FD7-46DC-9F9A-0AB6F6387CA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
   <si>
     <t>Nom de la Carte</t>
   </si>
@@ -339,6 +339,27 @@
   </si>
   <si>
     <t>Base Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Style 1</t>
+  </si>
+  <si>
+    <t>Style 2</t>
+  </si>
+  <si>
+    <t>IndValue</t>
+  </si>
+  <si>
+    <t>DistanceTarget</t>
+  </si>
+  <si>
+    <t>IndValueTarget</t>
+  </si>
+  <si>
+    <t>TargetNbr</t>
   </si>
 </sst>
 </file>
@@ -349,7 +370,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +421,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF954ECA"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -434,7 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,17 +533,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -648,6 +694,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF954ECA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -958,15 +1009,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04E4BE3-F23E-4EB7-8CE5-D09EE38FD482}">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="R70" sqref="R70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="7" width="7.5546875" customWidth="1"/>
     <col min="8" max="8" width="2.109375" style="2" customWidth="1"/>
@@ -1074,13 +1125,27 @@
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="I3" s="36">
+        <v>1</v>
+      </c>
+      <c r="J3" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="36">
+        <v>0.05</v>
+      </c>
+      <c r="L3" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="36">
+        <v>0.05</v>
+      </c>
+      <c r="N3" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="O3" s="36">
+        <v>0.01</v>
+      </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
       <c r="X3" s="13"/>
@@ -1316,6 +1381,12 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="Q9" s="4" t="s">
         <v>37</v>
       </c>
@@ -1338,6 +1409,17 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="39">
+        <f ca="1">((((($I$7+R12)*$I$3)/10)+(AVERAGE(T15,T16))*$J$3+(($K$7+R14)*($L$7+R15))*100*$K$3+(($M$7+R16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((R10/R11)*1000)*$L$3)-V11*2)/100</f>
+        <v>0.31225000000000003</v>
+      </c>
+      <c r="E10" s="39">
+        <f ca="1">((((($I$7+Y12)*$I$3)/10)+(AVERAGE(AA15,AA16))*$J$3+(($K$7+Y14)*($L$7+Y15))*100*$K$3+(($M$7+Y16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((Y10/Y11)*1000)*$L$3)-AC11*2)/100</f>
+        <v>0.35625000000000001</v>
+      </c>
       <c r="Q10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1362,10 +1444,19 @@
       </c>
       <c r="AA10" s="9">
         <f ca="1">((RANDBETWEEN($AA$6,$AC$6))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$7,$AC$7))+((($D$2*(1+($B$2/10))+10)/10))+((RANDBETWEEN($AA$8,$AC$8))+((($F$2*(1+($B$2/10))+10)/10))))</f>
-        <v>27.299999999999997</v>
+        <v>28.299999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>47</v>
       </c>
@@ -1406,6 +1497,15 @@
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="30">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30">
+        <v>1</v>
+      </c>
       <c r="Q12" s="4" t="s">
         <v>48</v>
       </c>
@@ -1432,6 +1532,9 @@
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C13" s="37"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="Q13" s="4" t="s">
         <v>49</v>
       </c>
@@ -1452,10 +1555,21 @@
       </c>
       <c r="AA13" s="18">
         <f ca="1">AA10*10</f>
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C14" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="38">
+        <f ca="1">D10+(-2.8*(D12/10*D12/10)+0.728)+(-0.0375*(D11^5)+0.470833333*(D11^4)-2.0375*(D11^3)+3.3291666667*(D11^2)-1.325*D11)</f>
+        <v>1.0122499999999999</v>
+      </c>
+      <c r="E14" s="38">
+        <f ca="1">E10+(-2.8*(E12/10*E12/10)+0.728)+(-0.0375*(E11^5)+0.470833333*(E11^4)-2.0375*(E11^3)+3.3291666667*(E11^2)-1.325*E11)</f>
+        <v>1.0562499999999999</v>
+      </c>
       <c r="Q14" s="4" t="s">
         <v>50</v>
       </c>
@@ -1476,10 +1590,13 @@
       </c>
       <c r="AA14" s="17">
         <f ca="1">AA10*($J$7+$Y$13)</f>
-        <v>40.949999999999996</v>
+        <v>42.449999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
       <c r="Q15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1769,7 +1886,7 @@
       </c>
       <c r="T23" s="9">
         <f ca="1">((RANDBETWEEN($T$19,$V$19))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
       <c r="X23" s="4" t="s">
         <v>46</v>
@@ -1782,7 +1899,7 @@
       </c>
       <c r="AA23" s="9">
         <f ca="1">((RANDBETWEEN($AA$19,$AC$19))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$20,$AC$20))+((($E$2*(1+($B$2/10))+10)/10)))</f>
-        <v>11.2</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
@@ -1861,7 +1978,7 @@
       </c>
       <c r="T26" s="18">
         <f ca="1">T23*10</f>
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>49</v>
@@ -1872,7 +1989,7 @@
       </c>
       <c r="AA26" s="18">
         <f ca="1">AA23*10</f>
-        <v>112</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
@@ -1885,7 +2002,7 @@
       </c>
       <c r="T27" s="17">
         <f ca="1">T23*($J$20+$R$26)</f>
-        <v>3.55</v>
+        <v>4.05</v>
       </c>
       <c r="X27" s="4" t="s">
         <v>50</v>
@@ -1898,7 +2015,7 @@
       </c>
       <c r="AA27" s="17">
         <f ca="1">AA23*($J$20+$Y$26)</f>
-        <v>5.6</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
@@ -2210,7 +2327,7 @@
       </c>
       <c r="AA36" s="9">
         <f ca="1">((RANDBETWEEN($AA$33,$AC$33))+((($F$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$32,$AC$32))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>6.2</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
@@ -2300,7 +2417,7 @@
       </c>
       <c r="AA39" s="18">
         <f ca="1">AA36*10</f>
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
@@ -2324,7 +2441,7 @@
       </c>
       <c r="AA40" s="17">
         <f ca="1">AA36*($J$33+$Y$39)</f>
-        <v>6.2</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
@@ -2619,7 +2736,7 @@
       </c>
       <c r="T49" s="9">
         <f ca="1">((RANDBETWEEN($T$46,$V$46))+((($E$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($T$45,$V$45))+((($F$2*(1+($B$2/10))+10)/10)))</f>
-        <v>8.1999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="X49" s="4" t="s">
         <v>46</v>
@@ -2632,7 +2749,7 @@
       </c>
       <c r="AA49" s="9">
         <f ca="1">((RANDBETWEEN($AA$46,$AC$46))+((($E$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$45,$AC$45))+((($F$2*(1+($B$2/10))+10)/10)))</f>
-        <v>16.2</v>
+        <v>18.2</v>
       </c>
       <c r="AC49" s="1"/>
     </row>
@@ -2713,7 +2830,7 @@
       </c>
       <c r="T52" s="18">
         <f ca="1">T49*10</f>
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="X52" s="4" t="s">
         <v>49</v>
@@ -2724,7 +2841,7 @@
       </c>
       <c r="AA52" s="18">
         <f ca="1">AA49*10</f>
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="AC52" s="1"/>
     </row>
@@ -2738,7 +2855,7 @@
       </c>
       <c r="T53" s="17">
         <f ca="1">T49*($J$46+$R$52)</f>
-        <v>16.399999999999999</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="X53" s="4" t="s">
         <v>50</v>
@@ -2751,7 +2868,7 @@
       </c>
       <c r="AA53" s="17">
         <f ca="1">AA49*($J$46+$Y$52)</f>
-        <v>32.4</v>
+        <v>36.4</v>
       </c>
       <c r="AC53" s="1"/>
     </row>
@@ -3067,7 +3184,7 @@
       </c>
       <c r="T62" s="9">
         <f ca="1">((RANDBETWEEN($T$59,$V$59))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($T$58,$V$58))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>20.2</v>
+        <v>22.2</v>
       </c>
       <c r="X62" s="4" t="s">
         <v>46</v>
@@ -3080,7 +3197,7 @@
       </c>
       <c r="AA62" s="9">
         <f ca="1">((RANDBETWEEN($AA$61,$AC$61))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$60,$AC$60))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$59,$AC$59))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$58,$AC$58))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>47.4</v>
+        <v>51.4</v>
       </c>
       <c r="AC62" s="1"/>
     </row>
@@ -3163,7 +3280,7 @@
       </c>
       <c r="T65" s="18">
         <f ca="1">T62*10</f>
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="X65" s="4" t="s">
         <v>49</v>
@@ -3176,7 +3293,7 @@
       </c>
       <c r="AA65" s="18">
         <f ca="1">AA62*10</f>
-        <v>474</v>
+        <v>514</v>
       </c>
       <c r="AC65" s="1"/>
     </row>
@@ -3190,7 +3307,7 @@
       </c>
       <c r="T66" s="17">
         <f ca="1">T62*($J$59+$R$65)</f>
-        <v>16.16</v>
+        <v>17.760000000000002</v>
       </c>
       <c r="X66" s="4" t="s">
         <v>50</v>
@@ -3203,7 +3320,7 @@
       </c>
       <c r="AA66" s="17">
         <f ca="1">AA62*($Y$65+$J$59)</f>
-        <v>47.4</v>
+        <v>51.4</v>
       </c>
       <c r="AC66" s="1"/>
     </row>
@@ -3293,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642083B0-1514-4BA4-9347-0B79E0A04B5F}">
   <dimension ref="B1:Z39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3324,16 +3441,16 @@
         <v>86</v>
       </c>
       <c r="E2" s="24"/>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
       <c r="N2" s="27" t="s">
         <v>95</v>
       </c>
@@ -3356,28 +3473,28 @@
       <c r="Z2" s="29"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="35">
         <f ca="1">AVERAGE((O3-$O$36),(P3-$P$36),(Q3-$Q$36),(R3-$R$36),(S3-$S$36),(O4-$O$37),(P4-$P$37),(Q4-$Q$37),(R4-$R$37),(S4-$S$37))</f>
         <v>0.30535999999999996</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E3" s="23"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33">
         <v>1.5</v>
       </c>
       <c r="O3" s="26">
@@ -3408,19 +3525,19 @@
       <c r="Z3" s="29"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="23"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
       <c r="O4" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+((Units!AA16)*N3)*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.5285000000000002</v>
@@ -3449,28 +3566,28 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="35">
         <f ca="1">AVERAGE((O5-$O$36),(P5-$P$36),(Q5-$Q$36),(R5-$R$36),(S5-$S$36),(O6-$O$37),(P6-$P$37),(Q6-$Q$37),(R6-$R$37),(S6-$S$37))</f>
         <v>0.29399999999999993</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>91</v>
       </c>
       <c r="E5" s="23"/>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33">
         <v>1.8</v>
       </c>
       <c r="O5" s="26">
@@ -3501,19 +3618,19 @@
       <c r="Z5" s="29"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
       <c r="O6" s="26">
         <f ca="1">((((((Units!$I$7+Units!Y12)*N5)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>1.9989999999999997</v>
@@ -3542,28 +3659,28 @@
       <c r="Z6" s="29"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="35">
         <f ca="1">AVERAGE((O7-$O$36),(P7-$P$36),(Q7-$Q$36),(R7-$R$36),(S7-$S$36),(O8-$O$37),(P8-$P$37),(Q8-$Q$37),(R8-$R$37),(S8-$S$37))</f>
         <v>0.438</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="33" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="31">
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34">
         <v>0.3</v>
       </c>
       <c r="O7" s="26">
@@ -3594,19 +3711,19 @@
       <c r="Z7" s="29"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
       <c r="O8" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14+N7)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.359</v>
@@ -3635,26 +3752,26 @@
       <c r="Z8" s="29"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="35">
         <f ca="1">AVERAGE((O9-$O$36),(P9-$P$36),(Q9-$Q$36),(R9-$R$36),(S9-$S$36),(O10-$O$37),(P10-$P$37),(Q10-$Q$37),(R10-$R$37),(S10-$S$37))</f>
         <v>0.4</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="33" t="s">
         <v>57</v>
       </c>
       <c r="E9" s="23"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="31">
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34">
         <v>0.5</v>
       </c>
       <c r="O9" s="26">
@@ -3685,19 +3802,19 @@
       <c r="Z9" s="29"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="30"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
       <c r="O10" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16+N9)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.2789999999999999</v>
@@ -3729,14 +3846,14 @@
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
       <c r="N11" s="7"/>
       <c r="W11" s="29"/>
       <c r="Y11" s="29"/>
@@ -3746,14 +3863,14 @@
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="7"/>
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
@@ -3764,336 +3881,336 @@
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
       <c r="N26" s="7"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="7"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
       <c r="N30" s="7"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="7"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
       <c r="N32" s="7"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="7"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
       <c r="N34" s="7"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
       <c r="N35" s="7"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
       <c r="N36" s="7"/>
       <c r="O36" s="26">
         <f ca="1">(((((Units!$I$7+Units!R12)*Units!$I$2)/10)+(AVERAGE(Units!T15,Units!T16))*Units!$J$2+((Units!$K$7+Units!R14)*(Units!$L$7+Units!R15))*100*Units!$K$2+((Units!$M$7+Units!R16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!R10/Units!R11)*1000)*Units!$L$2)-Units!V11*2)/100</f>
@@ -4147,21 +4264,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="F11:M11"/>
-    <mergeCell ref="F12:M12"/>
-    <mergeCell ref="F13:M13"/>
-    <mergeCell ref="F14:M14"/>
-    <mergeCell ref="F15:M15"/>
-    <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F26:M26"/>
-    <mergeCell ref="F27:M27"/>
-    <mergeCell ref="F16:M16"/>
-    <mergeCell ref="F17:M17"/>
-    <mergeCell ref="F18:M18"/>
-    <mergeCell ref="F19:M19"/>
-    <mergeCell ref="F20:M20"/>
-    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="F34:M34"/>
     <mergeCell ref="F35:M35"/>
     <mergeCell ref="F36:M36"/>
@@ -4178,22 +4296,21 @@
     <mergeCell ref="F22:M22"/>
     <mergeCell ref="F23:M23"/>
     <mergeCell ref="F24:M24"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="F15:M15"/>
+    <mergeCell ref="F25:M25"/>
+    <mergeCell ref="F26:M26"/>
+    <mergeCell ref="F27:M27"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="F17:M17"/>
+    <mergeCell ref="F18:M18"/>
+    <mergeCell ref="F19:M19"/>
+    <mergeCell ref="F20:M20"/>
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="F11:M11"/>
+    <mergeCell ref="F12:M12"/>
+    <mergeCell ref="F13:M13"/>
+    <mergeCell ref="F14:M14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="O3:S10">
@@ -4247,11 +4364,11 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -4260,9 +4377,9 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4284,15 +4401,15 @@
       </c>
       <c r="F7" s="8">
         <f ca="1">AVERAGE(F10:F110)</f>
-        <v>10.773267326732681</v>
+        <v>11.070297029702978</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" ref="G7:H7" ca="1" si="0">AVERAGE(G10:G110)</f>
-        <v>10.971287128712879</v>
+        <v>11.812871287128715</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8722772277227824</v>
+        <v>6.0702970297029815</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4324,15 +4441,15 @@
       </c>
       <c r="F10">
         <f ca="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
       <c r="G10">
         <f ca="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>12.1</v>
+        <v>6.1</v>
       </c>
       <c r="H10">
         <f ca="1">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4344,15 +4461,15 @@
       </c>
       <c r="F11">
         <f t="shared" ref="F11:G42" ca="1" si="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>7.1</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H74" ca="1" si="2">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
       <c r="N11" s="12"/>
     </row>
@@ -4365,25 +4482,25 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>6.1</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>12.1</v>
+        <v>15.1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>9.1</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
@@ -4393,19 +4510,19 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="9">
         <f ca="1">SUM(F7:H7)</f>
-        <v>27.616831683168343</v>
+        <v>28.953465346534674</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>9.1</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -4415,40 +4532,40 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>14.1</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>13.1</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E16" s="10"/>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>14.1</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>14.1</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
@@ -4466,67 +4583,67 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <f ca="1">10*C14</f>
-        <v>276.16831683168346</v>
+        <v>289.53465346534676</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
+        <v>9.1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
         <v>11.1</v>
       </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
-      </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>13.1</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
+        <v>10.1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="1"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="2"/>
         <v>7.1</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>11.1</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -4536,21 +4653,21 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>10.1</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
@@ -4560,21 +4677,21 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>14.1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>10.1</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
@@ -4582,101 +4699,101 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>14.1</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>12.1</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>14.1</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>15.1</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>9.1</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>11.1</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
@@ -4686,11 +4803,11 @@
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>14.1</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
@@ -4700,63 +4817,63 @@
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>12.1</v>
+        <v>11.1</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>7.1</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ca="1" si="1"/>
         <v>14.1</v>
       </c>
-      <c r="G37">
-        <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
-      </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>15.1</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>10.1</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
@@ -4764,13 +4881,13 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>11.1</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="1"/>
@@ -4778,69 +4895,69 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>15.1</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>12.1</v>
+        <v>15.1</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>7.1</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="43" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F43">
         <f t="shared" ref="F43:G74" ca="1" si="3">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="3"/>
+        <v>14.1</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ca="1" si="2"/>
         <v>9.1</v>
-      </c>
-      <c r="H43">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
       </c>
     </row>
     <row r="44" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F44">
         <f t="shared" ca="1" si="3"/>
+        <v>9.1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ca="1" si="3"/>
         <v>13.1</v>
       </c>
-      <c r="G44">
-        <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
-      </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F45">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>12.1</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="3"/>
@@ -4848,17 +4965,17 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="46" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F46">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>13.1</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
@@ -4868,25 +4985,25 @@
     <row r="47" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F47">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>15.1</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="48" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F48">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>13.1</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>15.1</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
@@ -4896,53 +5013,53 @@
     <row r="49" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F49">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F50">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>14.1</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F51">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>7.1</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F52">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
@@ -4952,25 +5069,25 @@
     <row r="53" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F53">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>12.1</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F54">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>14.1</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
@@ -4980,39 +5097,39 @@
     <row r="55" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F55">
         <f t="shared" ca="1" si="3"/>
+        <v>15.1</v>
+      </c>
+      <c r="G55">
+        <f t="shared" ca="1" si="3"/>
         <v>7.1</v>
       </c>
-      <c r="G55">
-        <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
-      </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="56" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F56">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="57" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F57">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
@@ -5022,11 +5139,11 @@
     <row r="58" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F58">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>14.1</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>7.1</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
@@ -5036,123 +5153,123 @@
     <row r="59" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F59">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>12.1</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="60" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F60">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="61" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F61">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="62" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F62">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>15.1</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>13.1</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="63" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F63">
         <f t="shared" ca="1" si="3"/>
+        <v>9.1</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ca="1" si="3"/>
         <v>13.1</v>
       </c>
-      <c r="G63">
-        <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
-      </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="64" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F64">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="65" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F65">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="66" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F66">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>12.1</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="67" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F67">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="2"/>
@@ -5162,15 +5279,15 @@
     <row r="68" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F68">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>14.1</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="69" spans="6:8" x14ac:dyDescent="0.3">
@@ -5180,67 +5297,67 @@
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>15.1</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="70" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F70">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>13.1</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="71" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F71">
         <f t="shared" ca="1" si="3"/>
+        <v>13.1</v>
+      </c>
+      <c r="G71">
+        <f t="shared" ca="1" si="3"/>
         <v>14.1</v>
       </c>
-      <c r="G71">
-        <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
-      </c>
       <c r="H71">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="72" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F72">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="3"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H72">
+        <f t="shared" ca="1" si="2"/>
         <v>9.1</v>
-      </c>
-      <c r="H72">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="73" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F73">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>14.1</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>11.1</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="74" spans="6:8" x14ac:dyDescent="0.3">
@@ -5250,17 +5367,17 @@
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="75" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F75">
         <f t="shared" ref="F75:G110" ca="1" si="4">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="4"/>
@@ -5268,31 +5385,31 @@
       </c>
       <c r="H75">
         <f t="shared" ref="H75:H110" ca="1" si="5">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="76" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F76">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="77" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F77">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="5"/>
@@ -5302,25 +5419,25 @@
     <row r="78" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F78">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>7.1</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="79" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F79">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="5"/>
@@ -5334,11 +5451,11 @@
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="81" spans="6:8" x14ac:dyDescent="0.3">
@@ -5352,17 +5469,17 @@
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="82" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F82">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="5"/>
@@ -5372,11 +5489,11 @@
     <row r="83" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F83">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>6.1</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="5"/>
@@ -5386,7 +5503,7 @@
     <row r="84" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F84">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="4"/>
@@ -5394,73 +5511,73 @@
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="85" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F85">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>15.1</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="86" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F86">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>14.1</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="87" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F87">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>7.1</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="88" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F88">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>9.1</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="89" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F89">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>7.1</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="5"/>
@@ -5470,43 +5587,43 @@
     <row r="90" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F90">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F91">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="92" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F92">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="93" spans="6:8" x14ac:dyDescent="0.3">
@@ -5516,161 +5633,161 @@
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="94" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F94">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>6.1</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>12.1</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="95" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F95">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="96" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F96">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>10.1</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="97" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F97">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>14.1</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="98" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F98">
         <f t="shared" ca="1" si="4"/>
+        <v>7.1</v>
+      </c>
+      <c r="G98">
+        <f t="shared" ca="1" si="4"/>
         <v>11.1</v>
-      </c>
-      <c r="G98">
-        <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="99" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F99">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="100" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F100">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>11.1</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>6.1</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="101" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F101">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>6.1</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="102" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F102">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="103" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F103">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="104" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F104">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>7.1</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>13.1</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="5"/>
@@ -5680,7 +5797,7 @@
     <row r="105" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F105">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>15.1</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="4"/>
@@ -5688,45 +5805,45 @@
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="106" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F106">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>15.1</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>14.1</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="107" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F107">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="108" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F108">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>11.1</v>
       </c>
       <c r="G108">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>11.1</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="5"/>
@@ -5736,29 +5853,29 @@
     <row r="109" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F109">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="G109">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="110" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F110">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>13.1</v>
       </c>
       <c r="G110">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>15.1</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -5771,21 +5888,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F72A5DAE2341648978EF9084C2699FE" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="39abd1a780d6cb1a58c150681616b65c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c2f5b03c-1842-4306-89f8-0f134e2596ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16b9d63b312e8e379de1a3d334a1c2af" ns3:_="">
     <xsd:import namespace="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
@@ -5931,31 +6033,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4B2B3B-C147-4047-A17B-E322C4A97431}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B0C01E-DDEA-436A-B152-B59D88A76C9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09B1061-3EAD-43E6-9035-9BD9BD8F789D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5971,4 +6064,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B0C01E-DDEA-436A-B152-B59D88A76C9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4B2B3B-C147-4047-A17B-E322C4A97431}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
First Expand Unit Value Factor
</commit_message>
<xml_diff>
--- a/GD-Docs/CodeCamelUnitProto.xlsx
+++ b/GD-Docs/CodeCamelUnitProto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phile\Documents\GitKraken\CodeCamelV2\GD-Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE902553-4E9F-45BF-8C8B-00334AC26186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF779F0-CE48-4A0C-BD19-AEF41F481A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11988" yWindow="1728" windowWidth="11268" windowHeight="8964" xr2:uid="{6B6672DD-3FD7-46DC-9F9A-0AB6F6387CA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B6672DD-3FD7-46DC-9F9A-0AB6F6387CA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="123">
   <si>
     <t>Nom de la Carte</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Base Style</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Style 1</t>
   </si>
   <si>
@@ -360,6 +357,57 @@
   </si>
   <si>
     <t>TargetNbr</t>
+  </si>
+  <si>
+    <t>Normalize</t>
+  </si>
+  <si>
+    <t>ValueTarget</t>
+  </si>
+  <si>
+    <t>Unit 1</t>
+  </si>
+  <si>
+    <t>Unit 2</t>
+  </si>
+  <si>
+    <t>Unit 3</t>
+  </si>
+  <si>
+    <t>Unit 4</t>
+  </si>
+  <si>
+    <t>Unit 5</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>U2S1</t>
+  </si>
+  <si>
+    <t>U4S2</t>
+  </si>
+  <si>
+    <t>U5S1</t>
+  </si>
+  <si>
+    <t>U2S2</t>
+  </si>
+  <si>
+    <t>U3S1</t>
+  </si>
+  <si>
+    <t>U4S1</t>
   </si>
 </sst>
 </file>
@@ -370,7 +418,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,8 +483,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF954ECA"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +511,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -469,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -533,11 +595,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,12 +614,28 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,7 +643,267 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="7" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill type="path">
@@ -1007,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04E4BE3-F23E-4EB7-8CE5-D09EE38FD482}">
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AN68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL23" sqref="AL23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,11 +1378,13 @@
     <col min="27" max="28" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1079,11 +1423,13 @@
       <c r="Q1" s="13"/>
       <c r="X1" s="13"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="42">
+        <v>0</v>
+      </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -1122,35 +1468,38 @@
       <c r="Q2" s="13"/>
       <c r="X2" s="13"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="36">
+      <c r="I3" s="40">
         <v>1</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="40">
         <v>0.5</v>
       </c>
-      <c r="K3" s="36">
+      <c r="K3" s="40">
         <v>0.05</v>
       </c>
-      <c r="L3" s="36">
+      <c r="L3" s="40">
         <v>0.1</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="40">
         <v>0.05</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="40">
         <v>0.2</v>
       </c>
-      <c r="O3" s="36">
+      <c r="O3" s="40">
         <v>0.01</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
@@ -1164,7 +1513,7 @@
       <c r="Q4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
@@ -1235,8 +1584,24 @@
         <f ca="1">((((($I$7+Y12)*$I$2)/10)+(AVERAGE(AA15,AA16))*$J$2+(($K$7+Y14)*($L$7+Y15))*100*$K$2+(($M$7+Y16)*$M$2)*100+$N$7*$N$2*10+$O$7*$O$2*10+((Y10/Y11)*1000)*$L$2)-AC11*2)/100</f>
         <v>1.879</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="Q6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1273,8 +1638,28 @@
       <c r="AC6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="44">
+        <f ca="1">D16</f>
+        <v>1.0122499999999999</v>
+      </c>
+      <c r="AJ6" s="45">
+        <f ca="1">E16</f>
+        <v>1.0562499999999999</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM6" s="31">
+        <v>150</v>
+      </c>
+      <c r="AN6" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f ca="1">MEDIAN(U5,AB5)</f>
         <v>1.6324999999999998</v>
@@ -1349,8 +1734,32 @@
       <c r="AC7" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI7" s="45">
+        <f ca="1">D29</f>
+        <v>1.2417500000000001</v>
+      </c>
+      <c r="AJ7" s="44">
+        <f ca="1">E29</f>
+        <v>1.4756666666666667</v>
+      </c>
+      <c r="AL7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM7" s="31">
+        <v>500</v>
+      </c>
+      <c r="AN7" s="31">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="I8" s="41">
+        <f>AM6</f>
+        <v>150</v>
+      </c>
       <c r="Q8" s="4" t="s">
         <v>36</v>
       </c>
@@ -1379,13 +1788,37 @@
       <c r="AC8" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI8" s="45">
+        <f ca="1">D42</f>
+        <v>0.95491666666666664</v>
+      </c>
+      <c r="AJ8" s="44">
+        <f ca="1">E42</f>
+        <v>0.97825000000000006</v>
+      </c>
+      <c r="AL8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM8" s="31">
+        <v>100</v>
+      </c>
+      <c r="AN8" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>102</v>
+      <c r="I9" s="41">
+        <f>AN6</f>
+        <v>100</v>
       </c>
       <c r="Q9" s="4" t="s">
         <v>37</v>
@@ -1407,17 +1840,37 @@
         <v>45</v>
       </c>
       <c r="AC9" s="1"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI9" s="44">
+        <f ca="1">D55</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AJ9" s="45">
+        <f ca="1">E55</f>
+        <v>0.99333333333333329</v>
+      </c>
+      <c r="AL9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM9" s="31">
+        <v>100</v>
+      </c>
+      <c r="AN9" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="39">
-        <f ca="1">((((($I$7+R12)*$I$3)/10)+(AVERAGE(T15,T16))*$J$3+(($K$7+R14)*($L$7+R15))*100*$K$3+(($M$7+R16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((R10/R11)*1000)*$L$3)-V11*2)/100</f>
+        <v>102</v>
+      </c>
+      <c r="D10" s="34">
+        <f ca="1">((((($I$8)*$I$3)/10)+(AVERAGE(T15,T16))*$J$3+(($K$7+R14)*($L$7+R15))*100*$K$3+(($M$7+R16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((R10/R11)*1000)*$L$3)-V11*2)/100</f>
         <v>0.31225000000000003</v>
       </c>
-      <c r="E10" s="39">
-        <f ca="1">((((($I$7+Y12)*$I$3)/10)+(AVERAGE(AA15,AA16))*$J$3+(($K$7+Y14)*($L$7+Y15))*100*$K$3+(($M$7+Y16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((Y10/Y11)*1000)*$L$3)-AC11*2)/100</f>
+      <c r="E10" s="34">
+        <f ca="1">((((($I$9)*$I$3)/10)+(AVERAGE(AA15,AA16))*$J$3+(($K$7+Y14)*($L$7+Y15))*100*$K$3+(($M$7+Y16)*$M$3)*100+$N$7*$N$3*10+$O$7*$O$3*10+((Y10/Y11)*1000)*$L$3)-AC11*2)/100</f>
         <v>0.35625000000000001</v>
       </c>
       <c r="Q10" s="4" t="s">
@@ -1444,17 +1897,39 @@
       </c>
       <c r="AA10" s="9">
         <f ca="1">((RANDBETWEEN($AA$6,$AC$6))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$7,$AC$7))+((($D$2*(1+($B$2/10))+10)/10))+((RANDBETWEEN($AA$8,$AC$8))+((($F$2*(1+($B$2/10))+10)/10))))</f>
-        <v>28.299999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+        <v>31.299999999999997</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI10" s="45">
+        <f ca="1">D68</f>
+        <v>1.1030500000000001</v>
+      </c>
+      <c r="AJ10" s="44">
+        <f ca="1">E68</f>
+        <v>1.18675</v>
+      </c>
+      <c r="AL10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM10" s="31">
+        <v>300</v>
+      </c>
+      <c r="AN10" s="31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="30">
+        <f>AM14</f>
         <v>0</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="31">
+        <f>AN14</f>
         <v>0</v>
       </c>
       <c r="Q11" s="4" t="s">
@@ -1496,14 +1971,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="30">
+        <f>AI14</f>
         <v>1</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="31">
+        <f>AJ14</f>
         <v>1</v>
       </c>
       <c r="Q12" s="4" t="s">
@@ -1531,8 +2008,8 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C13" s="37"/>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C13" s="32"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
       <c r="Q13" s="4" t="s">
@@ -1555,18 +2032,36 @@
       </c>
       <c r="AA13" s="18">
         <f ca="1">AA10*10</f>
-        <v>283</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C14" s="37" t="s">
+        <v>313</v>
+      </c>
+      <c r="AH13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="38">
+      <c r="AM13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN13" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C14" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="33">
         <f ca="1">D10+(-2.8*(D12/10*D12/10)+0.728)+(-0.0375*(D11^5)+0.470833333*(D11^4)-2.0375*(D11^3)+3.3291666667*(D11^2)-1.325*D11)</f>
         <v>1.0122499999999999</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="33">
         <f ca="1">E10+(-2.8*(E12/10*E12/10)+0.728)+(-0.0375*(E11^5)+0.470833333*(E11^4)-2.0375*(E11^3)+3.3291666667*(E11^2)-1.325*E11)</f>
         <v>1.0562499999999999</v>
       </c>
@@ -1590,13 +2085,28 @@
       </c>
       <c r="AA14" s="17">
         <f ca="1">AA10*($J$7+$Y$13)</f>
-        <v>42.449999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>100</v>
-      </c>
+        <v>46.949999999999996</v>
+      </c>
+      <c r="AH14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI14" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="Q15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1621,8 +2131,37 @@
         <f ca="1">AA11*($J$7+$Y$13)</f>
         <v>34.949999999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI15" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="43">
+        <f ca="1">(D14-$C$2)/($C$3-$C$2)</f>
+        <v>1.0122499999999999</v>
+      </c>
+      <c r="E16" s="43">
+        <f ca="1">(E14-$C$2)/($C$3-$C$2)</f>
+        <v>1.0562499999999999</v>
+      </c>
       <c r="Q16" s="4" t="s">
         <v>52</v>
       </c>
@@ -1647,8 +2186,46 @@
         <f ca="1">AA12*($J$7+$Y$13)</f>
         <v>49.949999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI16" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AH17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI17" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
@@ -1719,8 +2296,26 @@
         <f ca="1">((((($I$20+Y25)*$I$2)/10)+(AVERAGE(AA28,AA29))*$J$2+(($K$20+Y27)*($L$20+Y28))*100*$K$2+(($M$20+Y29)*$M$2)*100+$N$20*$N$2*10+$O$20*$O$2*10+((Y23/Y24)*1000)*$L$2)-AC24*2)/100</f>
         <v>1.8136666666666668</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI18" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ18" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="Q19" s="4" t="s">
         <v>34</v>
       </c>
@@ -1758,7 +2353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <f ca="1">MEDIAN(U18,AB18)</f>
         <v>1.5673333333333335</v>
@@ -1828,7 +2423,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="I21" s="41">
+        <f>AM7</f>
+        <v>500</v>
+      </c>
       <c r="Q21" s="4" t="s">
         <v>36</v>
       </c>
@@ -1851,8 +2450,24 @@
         <v>44</v>
       </c>
       <c r="AC21" s="1"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AH21" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI21" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="D22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="41">
+        <f>AN7</f>
+        <v>750</v>
+      </c>
       <c r="Q22" s="4" t="s">
         <v>37</v>
       </c>
@@ -1873,8 +2488,33 @@
         <v>45</v>
       </c>
       <c r="AC22" s="1"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AG22" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH22" s="42">
+        <f ca="1">AI7</f>
+        <v>1.2417500000000001</v>
+      </c>
+      <c r="AI22" s="42">
+        <f ca="1">AJ7</f>
+        <v>1.4756666666666667</v>
+      </c>
+      <c r="AJ22" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="34">
+        <f ca="1">((((($I$21)*$I$3)/10)+(AVERAGE(T28,T29))*$J$3+(($K$20+R27)*($L$20+R28))*100*$K$3+(($M$20+R29)*$M$3)*100+$N$20*$N$3*10+$O$20*$O$3*10+((R23/R24)*1000)*$L$3)-V24*2)/100</f>
+        <v>0.54175000000000006</v>
+      </c>
+      <c r="E23" s="34">
+        <f ca="1">((((($I$22)*$I$3)/10)+(AVERAGE(AA28,AA29))*$J$3+(($K$20+Y27)*($L$20+Y28))*100*$K$3+(($M$20+Y29)*$M$3)*100+$N$20*$N$3*10+$O$20*$O$3*10+((Y23/Y24)*1000)*$L$3)-AC24*2)/100</f>
+        <v>0.77566666666666662</v>
+      </c>
       <c r="Q23" s="4" t="s">
         <v>46</v>
       </c>
@@ -1886,7 +2526,7 @@
       </c>
       <c r="T23" s="9">
         <f ca="1">((RANDBETWEEN($T$19,$V$19))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="X23" s="4" t="s">
         <v>46</v>
@@ -1899,10 +2539,35 @@
       </c>
       <c r="AA23" s="9">
         <f ca="1">((RANDBETWEEN($AA$19,$AC$19))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$20,$AC$20))+((($E$2*(1+($B$2/10))+10)/10)))</f>
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+        <v>15.2</v>
+      </c>
+      <c r="AG23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AH23" s="42">
+        <f ca="1">AJ9</f>
+        <v>0.99333333333333329</v>
+      </c>
+      <c r="AI23" s="42">
+        <f ca="1">AI8</f>
+        <v>0.95491666666666664</v>
+      </c>
+      <c r="AJ23" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C24" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="31">
+        <f>AM15</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="31">
+        <f>AN15</f>
+        <v>0</v>
+      </c>
       <c r="Q24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1941,8 +2606,33 @@
       <c r="AC24" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AG24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH24" s="42">
+        <f ca="1">AI10</f>
+        <v>1.1030500000000001</v>
+      </c>
+      <c r="AI24" s="42">
+        <f ca="1">AI9</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AJ24" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="31">
+        <f>AI15</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="31">
+        <f>AJ15</f>
+        <v>1</v>
+      </c>
       <c r="Q25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1968,7 +2658,10 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C26" s="32"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
       <c r="Q26" s="4" t="s">
         <v>49</v>
       </c>
@@ -1978,7 +2671,7 @@
       </c>
       <c r="T26" s="18">
         <f ca="1">T23*10</f>
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>49</v>
@@ -1989,10 +2682,21 @@
       </c>
       <c r="AA26" s="18">
         <f ca="1">AA23*10</f>
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C27" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="33">
+        <f ca="1">D23+(-2.8*(D25/10*D25/10)+0.728)+(-0.0375*(D24^5)+0.470833333*(D24^4)-2.0375*(D24^3)+3.3291666667*(D24^2)-1.325*D24)</f>
+        <v>1.2417500000000001</v>
+      </c>
+      <c r="E27" s="33">
+        <f ca="1">E23+(-2.8*(E25/10*E25/10)+0.728)+(-0.0375*(E24^5)+0.470833333*(E24^4)-2.0375*(E24^3)+3.3291666667*(E24^2)-1.325*E24)</f>
+        <v>1.4756666666666667</v>
+      </c>
       <c r="Q27" s="4" t="s">
         <v>50</v>
       </c>
@@ -2002,7 +2706,7 @@
       </c>
       <c r="T27" s="17">
         <f ca="1">T23*($J$20+$R$26)</f>
-        <v>4.05</v>
+        <v>4.55</v>
       </c>
       <c r="X27" s="4" t="s">
         <v>50</v>
@@ -2015,10 +2719,10 @@
       </c>
       <c r="AA27" s="17">
         <f ca="1">AA23*($J$20+$Y$26)</f>
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="Q28" s="4" t="s">
         <v>51</v>
       </c>
@@ -2042,7 +2746,18 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="43">
+        <f ca="1">(D27-$C$2)/($C$3-$C$2)</f>
+        <v>1.2417500000000001</v>
+      </c>
+      <c r="E29" s="43">
+        <f ca="1">(E27-$C$2)/($C$3-$C$2)</f>
+        <v>1.4756666666666667</v>
+      </c>
       <c r="Q29" s="4" t="s">
         <v>52</v>
       </c>
@@ -2070,7 +2785,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -2142,7 +2857,7 @@
         <v>1.839</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="Q32" s="4" t="s">
         <v>34</v>
       </c>
@@ -2257,6 +2972,10 @@
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="I34" s="41">
+        <f>AM8</f>
+        <v>100</v>
+      </c>
       <c r="Q34" s="4" t="s">
         <v>36</v>
       </c>
@@ -2281,6 +3000,16 @@
       <c r="AC34" s="1"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="41">
+        <f>AN8</f>
+        <v>100</v>
+      </c>
       <c r="Q35" s="4" t="s">
         <v>37</v>
       </c>
@@ -2303,6 +3032,17 @@
       <c r="AC35" s="1"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="34">
+        <f ca="1">((((($I$34)*$I$3)/10)+(AVERAGE(T41,T42))*$J$3+(($K$33+R40)*($L$33+R41))*100*$K$3+(($M$33+R42)*$M$3)*100+$N$33*$N$3*10+$O$33*$O$3*10+((R36/R37)*1000)*$L$3)-V37*2)/100</f>
+        <v>0.25491666666666668</v>
+      </c>
+      <c r="E36" s="34">
+        <f ca="1">((((($I$35)*$I$3)/10)+(AVERAGE(AA41,AA42))*$J$3+(($K$33+Y40)*($L$33+Y41))*100*$K$3+(($M$33+Y42)*$M$3)*100+$N$33*$N$3*10+$O$33*$O$3*10+((Y36/Y37)*1000)*$L$3)-AC37*2)/100</f>
+        <v>0.27825000000000005</v>
+      </c>
       <c r="Q36" s="4" t="s">
         <v>46</v>
       </c>
@@ -2314,7 +3054,7 @@
       </c>
       <c r="T36" s="9">
         <f ca="1">((RANDBETWEEN($T$33,$V$33))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($T$32,$V$32))+((($F$2*(1+($B$2/10))+10)/10)))</f>
-        <v>11.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>46</v>
@@ -2327,10 +3067,21 @@
       </c>
       <c r="AA36" s="9">
         <f ca="1">((RANDBETWEEN($AA$33,$AC$33))+((($F$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$32,$AC$32))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>8.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="31">
+        <f>AM16</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="31">
+        <f>AN16</f>
+        <v>0</v>
+      </c>
       <c r="Q37" s="4" t="s">
         <v>47</v>
       </c>
@@ -2371,6 +3122,17 @@
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C38" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="31">
+        <f>AI16</f>
+        <v>1</v>
+      </c>
+      <c r="E38" s="31">
+        <f>AJ16</f>
+        <v>1</v>
+      </c>
       <c r="Q38" s="4" t="s">
         <v>48</v>
       </c>
@@ -2397,6 +3159,9 @@
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C39" s="32"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
       <c r="Q39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2406,7 +3171,7 @@
       </c>
       <c r="T39" s="18">
         <f ca="1">T36*10</f>
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>49</v>
@@ -2417,10 +3182,21 @@
       </c>
       <c r="AA39" s="18">
         <f ca="1">AA36*10</f>
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C40" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="33">
+        <f ca="1">D36+(-2.8*(D38/10*D38/10)+0.728)+(-0.0375*(D37^5)+0.470833333*(D37^4)-2.0375*(D37^3)+3.3291666667*(D37^2)-1.325*D37)</f>
+        <v>0.95491666666666664</v>
+      </c>
+      <c r="E40" s="33">
+        <f ca="1">E36+(-2.8*(E38/10*E38/10)+0.728)+(-0.0375*(E37^5)+0.470833333*(E37^4)-2.0375*(E37^3)+3.3291666667*(E37^2)-1.325*E37)</f>
+        <v>0.97825000000000006</v>
+      </c>
       <c r="Q40" s="4" t="s">
         <v>50</v>
       </c>
@@ -2430,7 +3206,7 @@
       </c>
       <c r="T40" s="17">
         <f ca="1">T36*($J$33+$R$39)</f>
-        <v>11.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="X40" s="4" t="s">
         <v>50</v>
@@ -2441,7 +3217,7 @@
       </c>
       <c r="AA40" s="17">
         <f ca="1">AA36*($J$33+$Y$39)</f>
-        <v>8.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
@@ -2469,6 +3245,17 @@
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="43">
+        <f ca="1">(D40-$C$2)/($C$3-$C$2)</f>
+        <v>0.95491666666666664</v>
+      </c>
+      <c r="E42" s="43">
+        <f ca="1">(E40-$C$2)/($C$3-$C$2)</f>
+        <v>0.97825000000000006</v>
+      </c>
       <c r="Q42" s="4" t="s">
         <v>52</v>
       </c>
@@ -2679,6 +3466,10 @@
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="I47" s="41">
+        <f>AM9</f>
+        <v>100</v>
+      </c>
       <c r="Q47" s="4" t="s">
         <v>36</v>
       </c>
@@ -2703,6 +3494,16 @@
       <c r="AC47" s="1"/>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I48" s="41">
+        <f>AN9</f>
+        <v>100</v>
+      </c>
       <c r="Q48" s="4" t="s">
         <v>37</v>
       </c>
@@ -2725,6 +3526,17 @@
       <c r="AC48" s="1"/>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C49" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="34">
+        <f ca="1">((((($I$47)*$I$3)/10)+(AVERAGE(T54,T55))*$J$3+(($K$46+R53)*($L$46+R54))*100*$K$3+(($M$46+R55)*$M$3)*100+$N$46*$N$3*10+$O$46*$O$3*10+((R49/R50)*1000)*$L$3)-V50*2)/100</f>
+        <v>0.245</v>
+      </c>
+      <c r="E49" s="34">
+        <f ca="1">((((($I$48)*$I$3)/10)+(AVERAGE(AA54,AA55))*$J$3+(($K$46+Y53)*($L$46+Y54))*100*$K$3+(($M$46+Y55)*$M$3)*100+$N$46*$N$3*10+$O$46*$O$3*10+((Y49/Y50)*1000)*$L$3)-AC50*2)/100</f>
+        <v>0.29333333333333333</v>
+      </c>
       <c r="Q49" s="4" t="s">
         <v>46</v>
       </c>
@@ -2736,7 +3548,7 @@
       </c>
       <c r="T49" s="9">
         <f ca="1">((RANDBETWEEN($T$46,$V$46))+((($E$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($T$45,$V$45))+((($F$2*(1+($B$2/10))+10)/10)))</f>
-        <v>9.1999999999999993</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="X49" s="4" t="s">
         <v>46</v>
@@ -2749,11 +3561,22 @@
       </c>
       <c r="AA49" s="9">
         <f ca="1">((RANDBETWEEN($AA$46,$AC$46))+((($E$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$45,$AC$45))+((($F$2*(1+($B$2/10))+10)/10)))</f>
-        <v>18.2</v>
+        <v>17.2</v>
       </c>
       <c r="AC49" s="1"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="31">
+        <f>AM17</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="31">
+        <f>AN17</f>
+        <v>0</v>
+      </c>
       <c r="Q50" s="4" t="s">
         <v>47</v>
       </c>
@@ -2794,6 +3617,17 @@
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C51" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="31">
+        <f>AI17</f>
+        <v>1</v>
+      </c>
+      <c r="E51" s="31">
+        <f>AJ17</f>
+        <v>1</v>
+      </c>
       <c r="Q51" s="4" t="s">
         <v>48</v>
       </c>
@@ -2821,6 +3655,9 @@
       <c r="AC51" s="1"/>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C52" s="32"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
       <c r="Q52" s="4" t="s">
         <v>49</v>
       </c>
@@ -2830,7 +3667,7 @@
       </c>
       <c r="T52" s="18">
         <f ca="1">T49*10</f>
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="X52" s="4" t="s">
         <v>49</v>
@@ -2841,11 +3678,22 @@
       </c>
       <c r="AA52" s="18">
         <f ca="1">AA49*10</f>
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="AC52" s="1"/>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C53" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="33">
+        <f ca="1">D49+(-2.8*(D51/10*D51/10)+0.728)+(-0.0375*(D50^5)+0.470833333*(D50^4)-2.0375*(D50^3)+3.3291666667*(D50^2)-1.325*D50)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="E53" s="33">
+        <f ca="1">E49+(-2.8*(E51/10*E51/10)+0.728)+(-0.0375*(E50^5)+0.470833333*(E50^4)-2.0375*(E50^3)+3.3291666667*(E50^2)-1.325*E50)</f>
+        <v>0.99333333333333329</v>
+      </c>
       <c r="Q53" s="4" t="s">
         <v>50</v>
       </c>
@@ -2855,7 +3703,7 @@
       </c>
       <c r="T53" s="17">
         <f ca="1">T49*($J$46+$R$52)</f>
-        <v>18.399999999999999</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="X53" s="4" t="s">
         <v>50</v>
@@ -2868,7 +3716,7 @@
       </c>
       <c r="AA53" s="17">
         <f ca="1">AA49*($J$46+$Y$52)</f>
-        <v>36.4</v>
+        <v>34.4</v>
       </c>
       <c r="AC53" s="1"/>
     </row>
@@ -2900,6 +3748,17 @@
       <c r="AC54" s="1"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="43">
+        <f ca="1">(D53-$C$2)/($C$3-$C$2)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="E55" s="43">
+        <f ca="1">(E53-$C$2)/($C$3-$C$2)</f>
+        <v>0.99333333333333329</v>
+      </c>
       <c r="Q55" s="4" t="s">
         <v>52</v>
       </c>
@@ -3113,6 +3972,10 @@
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="I60" s="41">
+        <f>AM10</f>
+        <v>300</v>
+      </c>
       <c r="Q60" s="4" t="s">
         <v>36</v>
       </c>
@@ -3143,6 +4006,16 @@
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" s="41">
+        <f>AN10</f>
+        <v>250</v>
+      </c>
       <c r="Q61" s="4" t="s">
         <v>37</v>
       </c>
@@ -3173,6 +4046,17 @@
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C62" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" s="34">
+        <f ca="1">((((($I$60)*$I$3)/10)+(AVERAGE(T67,T68))*$J$3+(($K$59+R66)*($L$59+R67))*100*$K$3+(($M$59+R68)*$M$3)*100+$N$59*$N$3*10+$O$59*$O$3*10+((R62/R63)*1000)*$L$3)-V63*2)/100</f>
+        <v>0.40305000000000002</v>
+      </c>
+      <c r="E62" s="34">
+        <f ca="1">((((($I$61)*$I$3)/10)+(AVERAGE(AA67,AA68))*$J$3+(($K$59+Y66)*($L$59+Y67))*100*$K$3+(($M$59+Y68)*$M$3)*100+$N$59*$N$3*10+$O$59*$O$3*10+((Y62/Y63)*1000)*$L$3)-AC63*2)/100</f>
+        <v>0.48675000000000002</v>
+      </c>
       <c r="Q62" s="4" t="s">
         <v>46</v>
       </c>
@@ -3184,7 +4068,7 @@
       </c>
       <c r="T62" s="9">
         <f ca="1">((RANDBETWEEN($T$59,$V$59))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($T$58,$V$58))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>22.2</v>
+        <v>19.2</v>
       </c>
       <c r="X62" s="4" t="s">
         <v>46</v>
@@ -3197,11 +4081,22 @@
       </c>
       <c r="AA62" s="9">
         <f ca="1">((RANDBETWEEN($AA$61,$AC$61))+((($D$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$60,$AC$60))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$59,$AC$59))+((($G$2*(1+($B$2/10))+10)/10)))+((RANDBETWEEN($AA$58,$AC$58))+((($G$2*(1+($B$2/10))+10)/10)))</f>
-        <v>51.4</v>
+        <v>50.4</v>
       </c>
       <c r="AC62" s="1"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="31">
+        <f>AM18</f>
+        <v>0</v>
+      </c>
+      <c r="E63" s="31">
+        <f>AN18</f>
+        <v>0</v>
+      </c>
       <c r="Q63" s="4" t="s">
         <v>47</v>
       </c>
@@ -3242,6 +4137,17 @@
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="C64" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="31">
+        <f>AI18</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="31">
+        <f>AJ18</f>
+        <v>1</v>
+      </c>
       <c r="Q64" s="4" t="s">
         <v>48</v>
       </c>
@@ -3270,7 +4176,10 @@
       </c>
       <c r="AC64" s="1"/>
     </row>
-    <row r="65" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="C65" s="32"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
       <c r="Q65" s="4" t="s">
         <v>49</v>
       </c>
@@ -3280,7 +4189,7 @@
       </c>
       <c r="T65" s="18">
         <f ca="1">T62*10</f>
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="X65" s="4" t="s">
         <v>49</v>
@@ -3293,11 +4202,22 @@
       </c>
       <c r="AA65" s="18">
         <f ca="1">AA62*10</f>
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="AC65" s="1"/>
     </row>
-    <row r="66" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="C66" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" s="33">
+        <f ca="1">D62+(-2.8*(D64/10*D64/10)+0.728)+(-0.0375*(D63^5)+0.470833333*(D63^4)-2.0375*(D63^3)+3.3291666667*(D63^2)-1.325*D63)</f>
+        <v>1.1030500000000001</v>
+      </c>
+      <c r="E66" s="33">
+        <f ca="1">E62+(-2.8*(E64/10*E64/10)+0.728)+(-0.0375*(E63^5)+0.470833333*(E63^4)-2.0375*(E63^3)+3.3291666667*(E63^2)-1.325*E63)</f>
+        <v>1.18675</v>
+      </c>
       <c r="Q66" s="4" t="s">
         <v>50</v>
       </c>
@@ -3307,7 +4227,7 @@
       </c>
       <c r="T66" s="17">
         <f ca="1">T62*($J$59+$R$65)</f>
-        <v>17.760000000000002</v>
+        <v>15.36</v>
       </c>
       <c r="X66" s="4" t="s">
         <v>50</v>
@@ -3320,11 +4240,11 @@
       </c>
       <c r="AA66" s="17">
         <f ca="1">AA62*($Y$65+$J$59)</f>
-        <v>51.4</v>
+        <v>50.4</v>
       </c>
       <c r="AC66" s="1"/>
     </row>
-    <row r="67" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:29" x14ac:dyDescent="0.3">
       <c r="Q67" s="4" t="s">
         <v>51</v>
       </c>
@@ -3349,7 +4269,18 @@
       </c>
       <c r="AC67" s="1"/>
     </row>
-    <row r="68" spans="17:29" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="C68" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="43">
+        <f ca="1">(D66-$C$2)/($C$3-$C$2)</f>
+        <v>1.1030500000000001</v>
+      </c>
+      <c r="E68" s="43">
+        <f ca="1">(E66-$C$2)/($C$3-$C$2)</f>
+        <v>1.18675</v>
+      </c>
       <c r="Q68" s="4" t="s">
         <v>52</v>
       </c>
@@ -3377,28 +4308,40 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C7">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Patate">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Patate">
       <formula>NOT(ISERROR(SEARCH("Patate",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Patate">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Patate">
       <formula>NOT(ISERROR(SEARCH("Patate",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Patate">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Patate">
       <formula>NOT(ISERROR(SEARCH("Patate",C33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Patate">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Patate">
       <formula>NOT(ISERROR(SEARCH("Patate",C46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Patate">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Patate">
       <formula>NOT(ISERROR(SEARCH("Patate",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI6:AJ10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3441,16 +4384,16 @@
         <v>86</v>
       </c>
       <c r="E2" s="24"/>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
       <c r="N2" s="27" t="s">
         <v>95</v>
       </c>
@@ -3473,28 +4416,28 @@
       <c r="Z2" s="29"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="37">
         <f ca="1">AVERAGE((O3-$O$36),(P3-$P$36),(Q3-$Q$36),(R3-$R$36),(S3-$S$36),(O4-$O$37),(P4-$P$37),(Q4-$Q$37),(R4-$R$37),(S4-$S$37))</f>
         <v>0.30535999999999996</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>89</v>
       </c>
       <c r="E3" s="23"/>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33">
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35">
         <v>1.5</v>
       </c>
       <c r="O3" s="26">
@@ -3525,19 +4468,19 @@
       <c r="Z3" s="29"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="23"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
       <c r="O4" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+((Units!AA16)*N3)*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.5285000000000002</v>
@@ -3566,28 +4509,28 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="37">
         <f ca="1">AVERAGE((O5-$O$36),(P5-$P$36),(Q5-$Q$36),(R5-$R$36),(S5-$S$36),(O6-$O$37),(P6-$P$37),(Q6-$Q$37),(R6-$R$37),(S6-$S$37))</f>
         <v>0.29399999999999993</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="35" t="s">
         <v>91</v>
       </c>
       <c r="E5" s="23"/>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35">
         <v>1.8</v>
       </c>
       <c r="O5" s="26">
@@ -3618,19 +4561,19 @@
       <c r="Z5" s="29"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
       <c r="O6" s="26">
         <f ca="1">((((((Units!$I$7+Units!Y12)*N5)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>1.9989999999999997</v>
@@ -3659,28 +4602,28 @@
       <c r="Z6" s="29"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="37">
         <f ca="1">AVERAGE((O7-$O$36),(P7-$P$36),(Q7-$Q$36),(R7-$R$36),(S7-$S$36),(O8-$O$37),(P8-$P$37),(Q8-$Q$37),(R8-$R$37),(S8-$S$37))</f>
         <v>0.438</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="35" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="34">
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36">
         <v>0.3</v>
       </c>
       <c r="O7" s="26">
@@ -3711,19 +4654,19 @@
       <c r="Z7" s="29"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B8" s="33"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="33"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14+N7)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.359</v>
@@ -3752,26 +4695,26 @@
       <c r="Z8" s="29"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="37">
         <f ca="1">AVERAGE((O9-$O$36),(P9-$P$36),(Q9-$Q$36),(R9-$R$36),(S9-$S$36),(O10-$O$37),(P10-$P$37),(Q10-$Q$37),(R10-$R$37),(S10-$S$37))</f>
         <v>0.4</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E9" s="23"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="34">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36">
         <v>0.5</v>
       </c>
       <c r="O9" s="26">
@@ -3802,19 +4745,19 @@
       <c r="Z9" s="29"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B10" s="33"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="33"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
       <c r="O10" s="26">
         <f ca="1">(((((Units!$I$7+Units!Y12)*Units!$I$2)/10)+(AVERAGE(Units!AA15,Units!AA16))*Units!$J$2+((Units!$K$7+Units!Y14)*(Units!$L$7+Units!Y15))*100*Units!$K$2+((Units!$M$7+Units!Y16+N9)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!Y10/Units!Y11)*1000)*Units!$L$2)-Units!AC11*2)/100</f>
         <v>2.2789999999999999</v>
@@ -3846,14 +4789,14 @@
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
       <c r="N11" s="7"/>
       <c r="W11" s="29"/>
       <c r="Y11" s="29"/>
@@ -3863,14 +4806,14 @@
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
       <c r="N12" s="7"/>
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
@@ -3881,336 +4824,336 @@
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
       <c r="N26" s="7"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
       <c r="N29" s="7"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
       <c r="N30" s="7"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
       <c r="N31" s="7"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
       <c r="N32" s="7"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
       <c r="N33" s="7"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
       <c r="N34" s="7"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
       <c r="N35" s="7"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
       <c r="N36" s="7"/>
       <c r="O36" s="26">
         <f ca="1">(((((Units!$I$7+Units!R12)*Units!$I$2)/10)+(AVERAGE(Units!T15,Units!T16))*Units!$J$2+((Units!$K$7+Units!R14)*(Units!$L$7+Units!R15))*100*Units!$K$2+((Units!$M$7+Units!R16)*Units!$M$2)*100+Units!$N$7*Units!$N$2*10+Units!$O$7*Units!$O$2*10+((Units!R10/Units!R11)*1000)*Units!$L$2)-Units!V11*2)/100</f>
@@ -4264,6 +5207,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="F11:M11"/>
+    <mergeCell ref="F12:M12"/>
+    <mergeCell ref="F13:M13"/>
+    <mergeCell ref="F14:M14"/>
+    <mergeCell ref="F15:M15"/>
+    <mergeCell ref="F25:M25"/>
+    <mergeCell ref="F26:M26"/>
+    <mergeCell ref="F27:M27"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="F17:M17"/>
+    <mergeCell ref="F18:M18"/>
+    <mergeCell ref="F19:M19"/>
+    <mergeCell ref="F20:M20"/>
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="F34:M34"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="F36:M36"/>
+    <mergeCell ref="F3:M4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F5:M6"/>
+    <mergeCell ref="F7:M8"/>
+    <mergeCell ref="F28:M28"/>
+    <mergeCell ref="F29:M29"/>
+    <mergeCell ref="F30:M30"/>
+    <mergeCell ref="F31:M31"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="F33:M33"/>
+    <mergeCell ref="F22:M22"/>
+    <mergeCell ref="F23:M23"/>
+    <mergeCell ref="F24:M24"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="N7:N8"/>
@@ -4280,37 +5254,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="F36:M36"/>
-    <mergeCell ref="F3:M4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F5:M6"/>
-    <mergeCell ref="F7:M8"/>
-    <mergeCell ref="F28:M28"/>
-    <mergeCell ref="F29:M29"/>
-    <mergeCell ref="F30:M30"/>
-    <mergeCell ref="F31:M31"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="F33:M33"/>
-    <mergeCell ref="F22:M22"/>
-    <mergeCell ref="F23:M23"/>
-    <mergeCell ref="F24:M24"/>
-    <mergeCell ref="F15:M15"/>
-    <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F26:M26"/>
-    <mergeCell ref="F27:M27"/>
-    <mergeCell ref="F16:M16"/>
-    <mergeCell ref="F17:M17"/>
-    <mergeCell ref="F18:M18"/>
-    <mergeCell ref="F19:M19"/>
-    <mergeCell ref="F20:M20"/>
-    <mergeCell ref="F21:M21"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="F11:M11"/>
-    <mergeCell ref="F12:M12"/>
-    <mergeCell ref="F13:M13"/>
-    <mergeCell ref="F14:M14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="O3:S10">
@@ -4364,11 +5307,11 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -4377,9 +5320,9 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4401,15 +5344,15 @@
       </c>
       <c r="F7" s="8">
         <f ca="1">AVERAGE(F10:F110)</f>
-        <v>11.070297029702978</v>
+        <v>11.208910891089115</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" ref="G7:H7" ca="1" si="0">AVERAGE(G10:G110)</f>
-        <v>11.812871287128715</v>
+        <v>10.90198019801981</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0702970297029815</v>
+        <v>5.892079207920804</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4441,11 +5384,11 @@
       </c>
       <c r="F10">
         <f ca="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>7.1</v>
+        <v>12.1</v>
       </c>
       <c r="G10">
         <f ca="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>6.1</v>
+        <v>11.1</v>
       </c>
       <c r="H10">
         <f ca="1">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
@@ -4461,15 +5404,15 @@
       </c>
       <c r="F11">
         <f t="shared" ref="F11:G42" ca="1" si="1">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>8.1</v>
+        <v>12.1</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H74" ca="1" si="2">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
-        <v>3.1</v>
+        <v>7.1</v>
       </c>
       <c r="N11" s="12"/>
     </row>
@@ -4482,47 +5425,47 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1</v>
+        <v>10.1</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>14.1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>12.1</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="9">
         <f ca="1">SUM(F7:H7)</f>
-        <v>28.953465346534674</v>
+        <v>28.00297029702973</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>11.1</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>12.1</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -4532,54 +5475,54 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>12.1</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E16" s="10"/>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>8.1</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>15.1</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>11.1</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
@@ -4589,99 +5532,99 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <f ca="1">10*C14</f>
-        <v>289.53465346534676</v>
+        <v>280.02970297029731</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>13.1</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>13.1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>13.1</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>7.1</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>10.1</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>6.1</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>12.1</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
@@ -4695,115 +5638,115 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>12.1</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>14.1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>12.1</v>
+        <v>8.1</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1</v>
+        <v>12.1</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>15.1</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>9.1</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
@@ -4811,73 +5754,73 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>13.1</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>7.1</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>6.1</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>10.1</v>
+        <v>6.1</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>13.1</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
-        <v>14.1</v>
+        <v>7.1</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
@@ -4887,11 +5830,11 @@
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="1"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
@@ -4901,25 +5844,25 @@
     <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>9.1</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>16.100000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>15.1</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
@@ -4929,39 +5872,39 @@
     <row r="43" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F43">
         <f t="shared" ref="F43:G74" ca="1" si="3">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="44" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F44">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F45">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>10.1</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
@@ -4971,133 +5914,133 @@
     <row r="46" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F46">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>13.1</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F47">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="48" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F48">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>13.1</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F49">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>10.1</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F50">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>14.1</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>8.1</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F51">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F52">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="53" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F53">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F54">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>11.1</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="55" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F55">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>6.1</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="3"/>
@@ -5105,17 +6048,17 @@
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="56" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F56">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
@@ -5125,25 +6068,25 @@
     <row r="57" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F57">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>12.1</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="58" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F58">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>11.1</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>13.1</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
@@ -5153,25 +6096,25 @@
     <row r="59" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F59">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>9.1</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="60" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F60">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>9.1</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>13.1</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
@@ -5181,53 +6124,53 @@
     <row r="61" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F61">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>11.1</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="62" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F62">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>9.1</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="63" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F63">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="64" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F64">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1</v>
+        <v>13.1</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
@@ -5237,81 +6180,81 @@
     <row r="65" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F65">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="3"/>
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="66" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F66">
         <f t="shared" ca="1" si="3"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="67" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F67">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1</v>
+        <v>10.1</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="68" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F68">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>9.1</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="69" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F69">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="3"/>
-        <v>15.1</v>
+        <v>8.1</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="70" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F70">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>11.1</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>10.1</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="2"/>
@@ -5321,35 +6264,35 @@
     <row r="71" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F71">
         <f t="shared" ca="1" si="3"/>
-        <v>13.1</v>
+        <v>12.1</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>8.1</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="72" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F72">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>8.1</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="3"/>
-        <v>16.100000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="73" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F73">
         <f t="shared" ca="1" si="3"/>
-        <v>14.1</v>
+        <v>12.1</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="3"/>
@@ -5357,55 +6300,55 @@
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="74" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F74">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1</v>
+        <v>15.1</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="3"/>
-        <v>11.1</v>
+        <v>13.1</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="75" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F75">
         <f t="shared" ref="F75:G110" ca="1" si="4">((RANDBETWEEN($B$10,$C$10))+((($C$5*(1+($C$1/10))+10)/10)))</f>
-        <v>15.1</v>
+        <v>14.1</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="H75">
         <f t="shared" ref="H75:H110" ca="1" si="5">((RANDBETWEEN($B$12,$C$12))+((($C$4*(1+($C$1/10))+10)/10)))</f>
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="76" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F76">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>12.1</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="77" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F77">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="4"/>
@@ -5413,49 +6356,49 @@
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="78" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F78">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="79" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F79">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="80" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F80">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="81" spans="6:8" x14ac:dyDescent="0.3">
@@ -5465,35 +6408,35 @@
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>15.1</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="82" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F82">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>13.1</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="83" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F83">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>7.1</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>12.1</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="5"/>
@@ -5503,21 +6446,21 @@
     <row r="84" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F84">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>11.1</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>12.1</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="85" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F85">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="4"/>
@@ -5525,27 +6468,27 @@
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="86" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F86">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="87" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F87">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>12.1</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="4"/>
@@ -5553,49 +6496,49 @@
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="88" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F88">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>8.1</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="89" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F89">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>7.1</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>15.1</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="90" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F90">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>9.1</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="6:8" x14ac:dyDescent="0.3">
@@ -5605,31 +6548,31 @@
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>9.1</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="92" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F92">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>12.1</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>15.1</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="93" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F93">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>10.1</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="4"/>
@@ -5637,31 +6580,31 @@
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="94" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F94">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>9.1</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="95" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F95">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="5"/>
@@ -5671,29 +6614,29 @@
     <row r="96" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F96">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="97" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F97">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>11.1</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>9.1</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="98" spans="6:8" x14ac:dyDescent="0.3">
@@ -5703,49 +6646,49 @@
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>8.1</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="99" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F99">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>10.1</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="100" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F100">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="101" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F101">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1</v>
+        <v>13.1</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>6.1</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="5"/>
@@ -5759,63 +6702,63 @@
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>12.1</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="5"/>
-        <v>7.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="103" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F103">
         <f t="shared" ca="1" si="4"/>
-        <v>10.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="4"/>
-        <v>9.1</v>
+        <v>11.1</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="104" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F104">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>10.1</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="5"/>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="105" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F105">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>9.1</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="4"/>
-        <v>12.1</v>
+        <v>7.1</v>
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="5"/>
-        <v>9.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="106" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F106">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>7.1</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="5"/>
@@ -5825,11 +6768,11 @@
     <row r="107" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F107">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1</v>
+        <v>12.1</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="5"/>
@@ -5839,43 +6782,43 @@
     <row r="108" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F108">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
       <c r="G108">
         <f t="shared" ca="1" si="4"/>
-        <v>11.1</v>
+        <v>7.1</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="5"/>
-        <v>8.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="109" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F109">
         <f t="shared" ca="1" si="4"/>
-        <v>14.1</v>
+        <v>12.1</v>
       </c>
       <c r="G109">
         <f t="shared" ca="1" si="4"/>
-        <v>16.100000000000001</v>
+        <v>15.1</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="110" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F110">
         <f t="shared" ca="1" si="4"/>
-        <v>13.1</v>
+        <v>7.1</v>
       </c>
       <c r="G110">
         <f t="shared" ca="1" si="4"/>
-        <v>15.1</v>
+        <v>7.1</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -5888,6 +6831,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F72A5DAE2341648978EF9084C2699FE" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="39abd1a780d6cb1a58c150681616b65c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c2f5b03c-1842-4306-89f8-0f134e2596ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16b9d63b312e8e379de1a3d334a1c2af" ns3:_="">
     <xsd:import namespace="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
@@ -6033,22 +6991,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4B2B3B-C147-4047-A17B-E322C4A97431}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B0C01E-DDEA-436A-B152-B59D88A76C9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09B1061-3EAD-43E6-9035-9BD9BD8F789D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6064,28 +7031,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B0C01E-DDEA-436A-B152-B59D88A76C9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4B2B3B-C147-4047-A17B-E322C4A97431}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c2f5b03c-1842-4306-89f8-0f134e2596ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>